<commit_message>
Fixed the arm with a new component
</commit_message>
<xml_diff>
--- a/reBot model/reBot-NUC-gen4.xlsx
+++ b/reBot model/reBot-NUC-gen4.xlsx
@@ -2100,7 +2100,7 @@
         <v>8</v>
       </c>
       <c r="F14">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="66" customHeight="1">
@@ -2117,7 +2117,7 @@
         <v>8</v>
       </c>
       <c r="F15">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="66" customHeight="1">

</xml_diff>